<commit_message>
actualizaciones en shiny. falta dejar la base bien ordenada y con las categorías correctas para que encuentre al buscar por DNI.
</commit_message>
<xml_diff>
--- a/Trabajo práctico final/Limpieza de bases/2024 ADMISIÓN_LIMPIA.xlsx
+++ b/Trabajo práctico final/Limpieza de bases/2024 ADMISIÓN_LIMPIA.xlsx
@@ -5387,12 +5387,12 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No asignada</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No asignada</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -5465,7 +5465,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No asignada</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -7600,7 +7600,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>28/10/1998</t>
+          <t>22/03/2492116</t>
         </is>
       </c>
       <c r="L85">
@@ -7708,7 +7708,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>18/01/1971</t>
+          <t>26/01/92264</t>
         </is>
       </c>
       <c r="L86">
@@ -7816,7 +7816,7 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>17/02/1990</t>
+          <t>28/07/1741053</t>
         </is>
       </c>
       <c r="L87">
@@ -7914,7 +7914,7 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>05/05/1994</t>
+          <t>01/06/2104875</t>
         </is>
       </c>
       <c r="L88">
@@ -8027,7 +8027,7 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>03/02/1985</t>
+          <t>25/01/1305792</t>
         </is>
       </c>
       <c r="L89">
@@ -8130,7 +8130,7 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>22/05/2000</t>
+          <t>11/10/2627425</t>
         </is>
       </c>
       <c r="L90">
@@ -8218,7 +8218,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Presente</t>
+          <t>No asignada</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -8228,7 +8228,7 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>20/12/1996</t>
+          <t>17/05/2331968</t>
         </is>
       </c>
       <c r="L91">
@@ -8331,7 +8331,7 @@
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>30/06/1985</t>
+          <t>04/09/1340565</t>
         </is>
       </c>
       <c r="L92">
@@ -8424,7 +8424,7 @@
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>30/03/2004</t>
+          <t>13/06/2960495</t>
         </is>
       </c>
       <c r="L93">
@@ -8522,7 +8522,7 @@
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>16/04/1994</t>
+          <t>13/11/2100380</t>
         </is>
       </c>
       <c r="L94">
@@ -8630,7 +8630,7 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>15/08/1978</t>
+          <t>28/08/746575</t>
         </is>
       </c>
       <c r="L95">
@@ -8733,7 +8733,7 @@
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>31/12/2003</t>
+          <t>26/06/2939205</t>
         </is>
       </c>
       <c r="L96">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>13/10/1989</t>
+          <t>25/01/1711011</t>
         </is>
       </c>
       <c r="L97">
@@ -8914,7 +8914,7 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>19/04/2001</t>
+          <t>03/02/2705962</t>
         </is>
       </c>
       <c r="L98">

</xml_diff>